<commit_message>
Update the score calculator
</commit_message>
<xml_diff>
--- a/2024/Score/Calculator/Excel.xlsx
+++ b/2024/Score/Calculator/Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\IngeniumTeam\ingeniumteam.github.io\2024\Score\Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03014B0B-279F-4E0D-93CF-6D8B76CB2DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38610098-6888-42A4-A71B-DEF627F32F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,6 @@
     <t>Team 2</t>
   </si>
   <si>
-    <t>Plants</t>
-  </si>
-  <si>
-    <t>Plant</t>
-  </si>
-  <si>
     <t>Dans un pot</t>
   </si>
   <si>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>Présent dans une zone</t>
+  </si>
+  <si>
+    <t>Plante</t>
+  </si>
+  <si>
+    <t>Plantes</t>
   </si>
 </sst>
 </file>
@@ -194,6 +194,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -207,21 +222,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,7 +545,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,112 +563,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="A1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="F3" s="14" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="F3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="F4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="F5" s="16"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H5" s="5">
         <v>12</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="F6" s="16"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H6" s="5">
-        <v>12</v>
-      </c>
-      <c r="I6" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5">
         <v>9</v>
-      </c>
-      <c r="C7" s="5">
-        <v>12</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="16"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H7" s="5">
         <v>12</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -677,68 +677,68 @@
       </c>
       <c r="C8" s="6">
         <f>C6*3+C7+C5</f>
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="F8" s="17"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" s="6">
         <f>H6*3+H7+H5</f>
-        <v>60</v>
-      </c>
-      <c r="I8" s="17"/>
+        <v>24</v>
+      </c>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="F9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="A9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="F9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="F10" s="16"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H10" s="5">
         <v>3</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="F11" s="16"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H11" s="5">
         <v>3</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -750,7 +750,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="F12" s="17"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
@@ -758,39 +758,39 @@
         <f>H10*5+H11*5</f>
         <v>30</v>
       </c>
-      <c r="I12" s="17"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="F13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="A13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="F13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="F14" s="16"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H14" s="5">
-        <v>5</v>
-      </c>
-      <c r="I14" s="16"/>
+        <v>6</v>
+      </c>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -799,32 +799,32 @@
       </c>
       <c r="C15" s="6">
         <f>C14*5</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="F15" s="17"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" s="6">
         <f>H14*5</f>
-        <v>25</v>
-      </c>
-      <c r="I15" s="17"/>
+        <v>30</v>
+      </c>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="F16" s="15" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="F16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -832,17 +832,17 @@
         <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="F17" s="16"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H17" s="5">
-        <v>115</v>
-      </c>
-      <c r="I17" s="16"/>
+        <v>84</v>
+      </c>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -851,18 +851,18 @@
       </c>
       <c r="C18" s="5">
         <f>C21</f>
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="F18" s="16"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H18" s="5">
         <f>H21</f>
-        <v>115</v>
-      </c>
-      <c r="I18" s="16"/>
+        <v>84</v>
+      </c>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -874,7 +874,7 @@
         <v>20</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="F19" s="17"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="4" t="s">
         <v>2</v>
       </c>
@@ -882,21 +882,21 @@
         <f>IF(_xlfn.CEILING.MATH(20-IF(H17&gt;H18, H17-H18, H18-H17))&lt;0,0,_xlfn.CEILING.MATH(20-IF(H17&gt;=H18, H17-H18,H18-H17)))</f>
         <v>20</v>
       </c>
-      <c r="I19" s="17"/>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="F20" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="A20" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="F20" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
@@ -905,19 +905,19 @@
       </c>
       <c r="C21" s="6">
         <f>SUM(C8,C12,C15)</f>
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="17"/>
+      <c r="F21" s="11"/>
       <c r="G21" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H21" s="6">
         <f>SUM(H8,H12,H15)</f>
-        <v>115</v>
-      </c>
-      <c r="I21" s="17"/>
+        <v>84</v>
+      </c>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
@@ -926,19 +926,19 @@
       </c>
       <c r="C22" s="6">
         <f>C21+C19+1</f>
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="17"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" s="6">
         <f>H21+H19+1</f>
-        <v>136</v>
-      </c>
-      <c r="I22" s="17"/>
+        <v>105</v>
+      </c>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -946,10 +946,10 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>